<commit_message>
rstudio::conf() abstract submission update
</commit_message>
<xml_diff>
--- a/OSM project overview.xlsx
+++ b/OSM project overview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15810" windowWidth="15360" windowHeight="7020" tabRatio="776" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="16740" windowWidth="15360" windowHeight="7020" tabRatio="776" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PAPER TEMPLATE" sheetId="16" r:id="rId1"/>
@@ -109,18 +109,6 @@
     <t>ProjectDescription</t>
   </si>
   <si>
-    <t>Ellie Brewer</t>
-  </si>
-  <si>
-    <t>Tom Cook</t>
-  </si>
-  <si>
-    <t>Becky Symons</t>
-  </si>
-  <si>
-    <t>Erika Wolff</t>
-  </si>
-  <si>
     <t>Amy Cizik</t>
   </si>
   <si>
@@ -503,6 +491,18 @@
   </si>
   <si>
     <t>Primary responsibilities</t>
+  </si>
+  <si>
+    <t>Ellie B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Becky S. </t>
+  </si>
+  <si>
+    <t>Erika W.</t>
   </si>
 </sst>
 </file>
@@ -1681,10 +1681,10 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -1773,8 +1773,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,16 +1790,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G1" t="s">
         <v>18</v>
@@ -1807,19 +1807,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D2" s="18">
         <v>0.05</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -1827,67 +1827,67 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D3" s="18">
         <v>0.3</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D4" s="18">
         <v>0.2</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D5" s="18">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="18">
         <v>0</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="18">
         <v>0</v>
@@ -1912,49 +1912,49 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="18">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="18">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D10" s="18">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -2014,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -2032,7 +2032,7 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2058,10 +2058,10 @@
         <v>43465</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2069,19 +2069,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1">
         <v>43191</v>
@@ -2090,10 +2090,10 @@
         <v>43313</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2101,19 +2101,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1">
         <v>43282</v>
@@ -2122,10 +2122,10 @@
         <v>43344</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2133,19 +2133,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G5" s="1">
         <v>43344</v>
@@ -2154,10 +2154,10 @@
         <v>43465</v>
       </c>
       <c r="I5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2168,16 +2168,16 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G6" s="1">
         <v>43282</v>
@@ -2189,7 +2189,7 @@
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2200,16 +2200,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G7" s="1">
         <v>43282</v>
@@ -2221,7 +2221,7 @@
         <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2235,13 +2235,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G8" s="1">
         <v>43282</v>
@@ -2253,7 +2253,7 @@
         <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2286,117 +2286,117 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
       <c r="G1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" t="s">
         <v>123</v>
       </c>
-      <c r="D5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F5" t="s">
-        <v>127</v>
-      </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2431,13 +2431,13 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -2446,18 +2446,18 @@
         <v>23</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="12">
         <v>43221</v>
@@ -2472,28 +2472,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" s="8">
         <v>43282</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8">
         <v>43313</v>
@@ -2506,10 +2506,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C5" s="8">
         <v>43319</v>
@@ -2522,10 +2522,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" s="8">
         <v>43282</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7" s="8">
         <v>43313</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8" s="12">
         <v>43327</v>
@@ -2611,13 +2611,13 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -2626,7 +2626,7 @@
         <v>23</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H1" s="15">
         <v>43496</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>5</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4">
         <v>43296</v>
@@ -2672,10 +2672,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="4">
         <f>WORKDAY($H$1, -65)</f>
@@ -2689,10 +2689,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4">
         <v>43327</v>
@@ -2707,10 +2707,10 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C6" s="4">
         <f>WORKDAY($H$1, -60)</f>
@@ -2725,15 +2725,15 @@
       </c>
       <c r="F6" s="5"/>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" s="4">
         <f>WORKDAY($H$1, -55)</f>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4">
         <f>WORKDAY($H$1, -50)</f>
@@ -2770,10 +2770,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4">
         <f>WORKDAY($H$1, -45)</f>
@@ -2787,10 +2787,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4">
         <f>WORKDAY($H$1, -55)</f>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -2847,10 +2847,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="4">
         <f>WORKDAY($H$1, -35)</f>
@@ -2864,10 +2864,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4">
         <f>WORKDAY($H$1,-30)</f>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C15" s="4">
         <f>WORKDAY($H$1,-20)</f>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="4">
         <f>WORKDAY($H$1, -25)</f>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4">
         <f>WORKDAY($H$1,-20)</f>
@@ -2941,10 +2941,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4">
         <f>WORKDAY($H$1,-15)</f>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C19" s="4">
         <f>$H$1</f>
@@ -2978,10 +2978,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C20" s="4">
         <f>WORKDAY($H$1,-5)</f>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C21" s="4">
         <f>WORKDAY($H$1,-5)</f>
@@ -3015,10 +3015,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="4">
         <f>$H$1</f>
@@ -3070,13 +3070,13 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -3085,7 +3085,7 @@
         <v>23</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H1" s="15">
         <v>43434</v>
@@ -3093,10 +3093,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" s="21">
         <v>43283</v>
@@ -3105,16 +3105,16 @@
         <v>43294</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="21">
         <f>WORKDAY(D5,5)</f>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="4">
         <f>WORKDAY($H$1, -80)</f>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="16">
         <f>WORKDAY($H$1,-70)</f>
@@ -3168,10 +3168,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4">
         <f>WORKDAY($H$1, -60)</f>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C7" s="4">
         <f>WORKDAY($H$1, -60)</f>
@@ -3208,10 +3208,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8" s="4">
         <f>WORKDAY($H$1, -55)</f>
@@ -3228,10 +3228,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C9" s="4">
         <f>WORKDAY($H$1, -50)</f>
@@ -3248,10 +3248,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4">
         <f>WORKDAY($H$1, -50)</f>
@@ -3268,10 +3268,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11" s="4">
         <f>WORKDAY($H$1, -55)</f>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
@@ -3328,10 +3328,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4">
         <f>WORKDAY($H$1, -40)</f>
@@ -3348,10 +3348,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C15" s="4">
         <f>WORKDAY($H$1,-30)</f>
@@ -3368,10 +3368,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4">
         <f>WORKDAY($H$1,-25)</f>
@@ -3388,10 +3388,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4">
         <f>WORKDAY(D18, -25)</f>
@@ -3408,10 +3408,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4">
         <f>WORKDAY($H$1,-20)</f>
@@ -3428,10 +3428,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4">
         <f>WORKDAY($H$1,-20)</f>
@@ -3448,10 +3448,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="4">
         <f>WORKDAY($H$1,-15)</f>
@@ -3468,10 +3468,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C21" s="4">
         <f>WORKDAY($H$1,-10)</f>
@@ -3488,10 +3488,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="4">
         <f>WORKDAY($H$1,-5)</f>
@@ -3508,10 +3508,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C23" s="4">
         <f>WORKDAY($H$1,-5)</f>
@@ -3571,13 +3571,13 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
@@ -3609,7 +3609,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3624,19 +3624,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
@@ -3644,13 +3644,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D2" s="1">
         <v>43350</v>
@@ -3661,10 +3661,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -3678,10 +3678,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -3695,10 +3695,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -3712,13 +3712,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D6" s="1">
         <v>43343</v>
@@ -3729,13 +3729,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D7" s="1">
         <v>43357</v>
@@ -3746,10 +3746,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -3763,10 +3763,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -3780,10 +3780,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -3797,13 +3797,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D11" s="1">
         <v>43357</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -3831,13 +3831,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D13" s="1">
         <v>43405</v>
@@ -3848,10 +3848,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -3865,10 +3865,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -3882,10 +3882,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>6</v>

</xml_diff>